<commit_message>
Excel charts to have title.
</commit_message>
<xml_diff>
--- a/res/Data Quality Survey Recap.xlsx
+++ b/res/Data Quality Survey Recap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
@@ -381,6 +381,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -398,9 +401,6 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -599,7 +599,68 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Seberapa baik rute kami?</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-SG">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1009,11 +1070,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1496527184"/>
-        <c:axId val="1496529904"/>
+        <c:axId val="-929037712"/>
+        <c:axId val="-632319168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1496527184"/>
+        <c:axId val="-929037712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,7 +1173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1496529904"/>
+        <c:crossAx val="-632319168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1120,7 +1181,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1496529904"/>
+        <c:axId val="-632319168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1288,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1496527184"/>
+        <c:crossAx val="-929037712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1322,7 +1383,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Di mana Anda...?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1589,11 +1706,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1573070720"/>
-        <c:axId val="1573071264"/>
+        <c:axId val="-632322432"/>
+        <c:axId val="-632322976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1573070720"/>
+        <c:axId val="-632322432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,7 +1809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1573071264"/>
+        <c:crossAx val="-632322976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1700,7 +1817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1573071264"/>
+        <c:axId val="-632322976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +1924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1573070720"/>
+        <c:crossAx val="-632322432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1902,7 +2019,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Anda tertarik untuk kontribusi data rute?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -2183,7 +2356,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Seberapa baik rute kami?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2593,11 +2822,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1586155824"/>
-        <c:axId val="1586151472"/>
+        <c:axId val="-632314272"/>
+        <c:axId val="-632321344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1586155824"/>
+        <c:axId val="-632314272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2696,7 +2925,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1586151472"/>
+        <c:crossAx val="-632321344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2704,7 +2933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1586151472"/>
+        <c:axId val="-632321344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2811,7 +3040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1586155824"/>
+        <c:crossAx val="-632314272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2906,7 +3135,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Di mana Anda...?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3173,11 +3458,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1586155280"/>
-        <c:axId val="1586156912"/>
+        <c:axId val="-632313728"/>
+        <c:axId val="-632316448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1586155280"/>
+        <c:axId val="-632313728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3276,7 +3561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1586156912"/>
+        <c:crossAx val="-632316448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3284,7 +3569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1586156912"/>
+        <c:axId val="-632316448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3391,7 +3676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1586155280"/>
+        <c:crossAx val="-632313728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7032,15 +7317,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7062,15 +7347,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1681162</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:colOff>1509712</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7127,15 +7412,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7159,15 +7444,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1681162</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:colOff>1604962</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7243,13 +7528,13 @@
   <autoFilter ref="B36:E41"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Penilaian"/>
-    <tableColumn id="2" name="Keseluruhan" dataDxfId="19">
+    <tableColumn id="2" name="Keseluruhan" dataDxfId="20">
       <calculatedColumnFormula>COUNTIF(Table1[How good is our route? / Seberapa baik rute kami? '[Overall / Keseluruhan']],Table2[[#This Row],[Penilaian]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Rute kendaraan" dataDxfId="18">
+    <tableColumn id="3" name="Rute kendaraan" dataDxfId="19">
       <calculatedColumnFormula>COUNTIF(Table1[How good is our route? / Seberapa baik rute kami? '[Vehicle path / Rute kendaraan']],Table2[[#This Row],[Penilaian]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Rute berjalan" dataDxfId="17">
+    <tableColumn id="4" name="Rute berjalan" dataDxfId="18">
       <calculatedColumnFormula>COUNTIF(Table1[How good is our route? / Seberapa baik rute kami? '[Walking path / Rute berjalan']],Table2[[#This Row],[Penilaian]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7262,10 +7547,10 @@
   <autoFilter ref="E43:G47"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Kota"/>
-    <tableColumn id="2" name="Menggunakan KIRI" dataDxfId="20">
+    <tableColumn id="2" name="Menggunakan KIRI" dataDxfId="17">
       <calculatedColumnFormula>COUNTIF(Table1[Where do you use KIRI? / Di mana Anda menggunakan KIRI?], CONCATENATE("*", Table3[[#This Row],[Kota]], "*"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Tempat Tinggal" dataDxfId="15">
+    <tableColumn id="3" name="Tempat Tinggal" dataDxfId="16">
       <calculatedColumnFormula>COUNTIF(Table1[Where do you live mainly? / Di mana Anda tinggal?],Table3[[#This Row],[Kota]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7278,7 +7563,7 @@
   <autoFilter ref="G36:H40"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Interest"/>
-    <tableColumn id="2" name="Responden" dataDxfId="16">
+    <tableColumn id="2" name="Responden" dataDxfId="15">
       <calculatedColumnFormula>COUNTIF(Table1[Are you interested in contributing route data? / Anda tertarik untuk kontribusi data rute?],Table5[[#This Row],[Interest]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7616,9 +7901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8662,9 +8947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>